<commit_message>
Chore: updated code to use latest version of equilibrator (0.2.1b1)
</commit_message>
<xml_diff>
--- a/set_up_grasp_models/tests/test_files/test_set_up_models/set_up_model/true_res_model_v3.xlsx
+++ b/set_up_grasp_models/tests/test_files/test_set_up_models/set_up_model/true_res_model_v3.xlsx
@@ -16137,10 +16137,10 @@
         <v>70</v>
       </c>
       <c r="B3">
-        <v>-185.5</v>
+        <v>-184.66</v>
       </c>
       <c r="C3">
-        <v>-182.54</v>
+        <v>-183.06</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -16148,10 +16148,10 @@
         <v>71</v>
       </c>
       <c r="B4">
-        <v>-17.98</v>
+        <v>-17.67</v>
       </c>
       <c r="C4">
-        <v>-16.54</v>
+        <v>-16.79</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -16170,10 +16170,10 @@
         <v>73</v>
       </c>
       <c r="B6">
-        <v>-13.41</v>
+        <v>-13.28</v>
       </c>
       <c r="C6">
-        <v>-6.81</v>
+        <v>-6.720000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -16192,10 +16192,10 @@
         <v>75</v>
       </c>
       <c r="B8">
-        <v>-15.37</v>
+        <v>-15.53</v>
       </c>
       <c r="C8">
-        <v>0.2299999999999995</v>
+        <v>-8.449999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -16203,10 +16203,10 @@
         <v>76</v>
       </c>
       <c r="B9">
-        <v>-28.04</v>
+        <v>-18.47</v>
       </c>
       <c r="C9">
-        <v>-13.54</v>
+        <v>-14.65</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -16214,10 +16214,10 @@
         <v>77</v>
       </c>
       <c r="B10">
-        <v>-29.04</v>
+        <v>-19.27</v>
       </c>
       <c r="C10">
-        <v>-14.52</v>
+        <v>-15.39</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -16247,10 +16247,10 @@
         <v>80</v>
       </c>
       <c r="B13">
-        <v>-4.44</v>
+        <v>-3.75</v>
       </c>
       <c r="C13">
-        <v>-0.1999999999999997</v>
+        <v>-1.05</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -16258,10 +16258,10 @@
         <v>81</v>
       </c>
       <c r="B14">
-        <v>-5.45</v>
+        <v>-4.55</v>
       </c>
       <c r="C14">
-        <v>-1.17</v>
+        <v>-1.79</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -16269,10 +16269,10 @@
         <v>82</v>
       </c>
       <c r="B15">
-        <v>-4.44</v>
+        <v>-3.75</v>
       </c>
       <c r="C15">
-        <v>-0.1999999999999997</v>
+        <v>-1.05</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -16280,10 +16280,10 @@
         <v>83</v>
       </c>
       <c r="B16">
-        <v>-181.4</v>
+        <v>-180.32</v>
       </c>
       <c r="C16">
-        <v>-175.7</v>
+        <v>-176.72</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -16291,10 +16291,10 @@
         <v>84</v>
       </c>
       <c r="B17">
-        <v>2.58</v>
+        <v>7.049999999999999</v>
       </c>
       <c r="C17">
-        <v>17.78</v>
+        <v>13.53</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -16302,10 +16302,10 @@
         <v>85</v>
       </c>
       <c r="B18">
-        <v>3.56</v>
+        <v>7.83</v>
       </c>
       <c r="C18">
-        <v>18.78</v>
+        <v>14.31</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -16313,10 +16313,10 @@
         <v>86</v>
       </c>
       <c r="B19">
-        <v>-3.09</v>
+        <v>-2.7</v>
       </c>
       <c r="C19">
-        <v>-0.77</v>
+        <v>-1.14</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -16324,10 +16324,10 @@
         <v>87</v>
       </c>
       <c r="B20">
-        <v>-4.53</v>
+        <v>-4.56</v>
       </c>
       <c r="C20">
-        <v>-2.21</v>
+        <v>-2.2</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -16335,10 +16335,10 @@
         <v>88</v>
       </c>
       <c r="B21">
-        <v>-5.96</v>
+        <v>-5.890000000000001</v>
       </c>
       <c r="C21">
-        <v>-1.64</v>
+        <v>-1.97</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -16346,10 +16346,10 @@
         <v>89</v>
       </c>
       <c r="B22">
-        <v>-12.08</v>
+        <v>-11.95</v>
       </c>
       <c r="C22">
-        <v>-7.9</v>
+        <v>-8.030000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -16357,10 +16357,10 @@
         <v>90</v>
       </c>
       <c r="B23">
-        <v>-2.35</v>
+        <v>-2.02</v>
       </c>
       <c r="C23">
-        <v>0.8900000000000001</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -16368,10 +16368,10 @@
         <v>91</v>
       </c>
       <c r="B24">
-        <v>111.67</v>
+        <v>111.76</v>
       </c>
       <c r="C24">
-        <v>117.45</v>
+        <v>117.2</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -16379,10 +16379,10 @@
         <v>92</v>
       </c>
       <c r="B25">
-        <v>13.3</v>
+        <v>13.43</v>
       </c>
       <c r="C25">
-        <v>17.76</v>
+        <v>17.67</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -16390,10 +16390,10 @@
         <v>93</v>
       </c>
       <c r="B26">
-        <v>-3.13</v>
+        <v>-2.92</v>
       </c>
       <c r="C26">
-        <v>-1.93</v>
+        <v>-2.14</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -16401,10 +16401,10 @@
         <v>94</v>
       </c>
       <c r="B27">
-        <v>-170.65</v>
+        <v>-169.9</v>
       </c>
       <c r="C27">
-        <v>-167.47</v>
+        <v>-167.82</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -16412,10 +16412,10 @@
         <v>95</v>
       </c>
       <c r="B28">
-        <v>-20.67</v>
+        <v>-20.36</v>
       </c>
       <c r="C28">
-        <v>-18.93</v>
+        <v>-19.28</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -16423,10 +16423,10 @@
         <v>96</v>
       </c>
       <c r="B29">
-        <v>-6.23</v>
+        <v>-6</v>
       </c>
       <c r="C29">
-        <v>-4.73</v>
+        <v>-4.880000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -16434,10 +16434,10 @@
         <v>97</v>
       </c>
       <c r="B30">
-        <v>6.88</v>
+        <v>7.44</v>
       </c>
       <c r="C30">
-        <v>8.68</v>
+        <v>8.26</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -16445,10 +16445,10 @@
         <v>98</v>
       </c>
       <c r="B31">
-        <v>-19.34</v>
+        <v>-18.92</v>
       </c>
       <c r="C31">
-        <v>-17.56</v>
+        <v>-18.02</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -16456,10 +16456,10 @@
         <v>99</v>
       </c>
       <c r="B32">
-        <v>3.56</v>
+        <v>3.88</v>
       </c>
       <c r="C32">
-        <v>4.88</v>
+        <v>4.62</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -16467,10 +16467,10 @@
         <v>100</v>
       </c>
       <c r="B33">
-        <v>152.03</v>
+        <v>152.57</v>
       </c>
       <c r="C33">
-        <v>155.05</v>
+        <v>154.21</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -16478,10 +16478,10 @@
         <v>101</v>
       </c>
       <c r="B34">
-        <v>-28.62</v>
+        <v>-28.05</v>
       </c>
       <c r="C34">
-        <v>-26.74</v>
+        <v>-27.19</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -16489,10 +16489,10 @@
         <v>102</v>
       </c>
       <c r="B35">
-        <v>-318.11</v>
+        <v>-313.2</v>
       </c>
       <c r="C35">
-        <v>-302.01</v>
+        <v>-306.4</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -16500,10 +16500,10 @@
         <v>103</v>
       </c>
       <c r="B36">
-        <v>-19.4</v>
+        <v>-18.1</v>
       </c>
       <c r="C36">
-        <v>-15.44</v>
+        <v>-16.5</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -16511,10 +16511,10 @@
         <v>104</v>
       </c>
       <c r="B37">
-        <v>-185.5</v>
+        <v>-184.66</v>
       </c>
       <c r="C37">
-        <v>-182.54</v>
+        <v>-183.06</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -16522,10 +16522,10 @@
         <v>105</v>
       </c>
       <c r="B38">
-        <v>-65.11</v>
+        <v>-64.84</v>
       </c>
       <c r="C38">
-        <v>-63.17</v>
+        <v>-63.72</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -16533,10 +16533,10 @@
         <v>106</v>
       </c>
       <c r="B39">
-        <v>64.14</v>
+        <v>64.45</v>
       </c>
       <c r="C39">
-        <v>66.11999999999999</v>
+        <v>65.67</v>
       </c>
     </row>
     <row r="40" spans="1:3">

</xml_diff>